<commit_message>
Update Design decisions tracking.xlsx
</commit_message>
<xml_diff>
--- a/background_docs/Design decisions tracking.xlsx
+++ b/background_docs/Design decisions tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\COMP0022_Coursework\background_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AC1A454-2B39-4457-BBF3-043F8ED5D3C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEEB695-0F6C-412C-A1A0-64840F9858D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="R1" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="R6" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="21">
   <si>
     <t>example.php</t>
   </si>
@@ -152,6 +151,21 @@
   </si>
   <si>
     <t>Requirement 6</t>
+  </si>
+  <si>
+    <t>header.php</t>
+  </si>
+  <si>
+    <t>login_result.php</t>
+  </si>
+  <si>
+    <t>logout.php</t>
+  </si>
+  <si>
+    <t>process_registration.php</t>
+  </si>
+  <si>
+    <t>register.php</t>
   </si>
 </sst>
 </file>
@@ -583,20 +597,12 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>4</v>
-      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
       <c r="G5" s="5" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -605,7 +611,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="G6" s="5" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -613,7 +619,9 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
@@ -621,14 +629,18 @@
       <c r="C8" s="8"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
-      <c r="G8" s="5"/>
+      <c r="G8" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="7"/>

</xml_diff>

<commit_message>
Adding in standard db_credentials
</commit_message>
<xml_diff>
--- a/background_docs/Design decisions tracking.xlsx
+++ b/background_docs/Design decisions tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\COMP0022_Coursework\background_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEEB695-0F6C-412C-A1A0-64840F9858D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BADBDB-C904-46A6-B0E5-ED22ACD57445}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,9 +153,6 @@
     <t>Requirement 6</t>
   </si>
   <si>
-    <t>header.php</t>
-  </si>
-  <si>
     <t>login_result.php</t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t>register.php</t>
+  </si>
+  <si>
+    <t>php/check_username.php</t>
   </si>
 </sst>
 </file>
@@ -570,7 +570,7 @@
     <col min="3" max="3" width="33.7265625" customWidth="1"/>
     <col min="4" max="4" width="33.90625" customWidth="1"/>
     <col min="5" max="5" width="46.36328125" customWidth="1"/>
-    <col min="7" max="7" width="23.7265625" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.6">

</xml_diff>

<commit_message>
Removing 'browse' from main website, login fix
</commit_message>
<xml_diff>
--- a/background_docs/Design decisions tracking.xlsx
+++ b/background_docs/Design decisions tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\COMP0022_Coursework\background_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BADBDB-C904-46A6-B0E5-ED22ACD57445}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED44748-C5E5-4BA6-81DA-23BBAE7F4471}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="38">
   <si>
     <t>example.php</t>
   </si>
@@ -166,6 +166,57 @@
   </si>
   <si>
     <t>php/check_username.php</t>
+  </si>
+  <si>
+    <t>php/login_register_form_validation.php</t>
+  </si>
+  <si>
+    <t>Better user experience</t>
+  </si>
+  <si>
+    <t>Countries from drop-down menu, not user-inputted</t>
+  </si>
+  <si>
+    <t>Part of DB design</t>
+  </si>
+  <si>
+    <t>Password matching is only checked on client-side</t>
+  </si>
+  <si>
+    <t>Users who are submitting their own HTTP requests can deal with the inconvenience if it happens!</t>
+  </si>
+  <si>
+    <t>Use SQL function for the above</t>
+  </si>
+  <si>
+    <t>More robust since not part of a 'development environment'</t>
+  </si>
+  <si>
+    <t>Easier code readability</t>
+  </si>
+  <si>
+    <t>Check username uniqueness in real time using AJAX (&amp; before form submission)</t>
+  </si>
+  <si>
+    <t>Separate php file containing user input validation/sanitisation functions</t>
+  </si>
+  <si>
+    <t>If query for above fails, do not terminate registration form</t>
+  </si>
+  <si>
+    <t>Address data is optional, so give users the opportunity just to to submit it with their current registration form (or try to refresh)</t>
+  </si>
+  <si>
+    <t>Same for checking username uniqueness - though they can't submit the form unless the check works</t>
+  </si>
+  <si>
+    <t>The query will keep on being tried each time focus is lost on the username input field, so it might work again in the future (e.g. a temporary connection glitch)</t>
+  </si>
+  <si>
+    <t>Validate/sanitise all user input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard reasons - client-side protections are not robust </t>
   </si>
 </sst>
 </file>
@@ -570,7 +621,7 @@
     <col min="3" max="3" width="33.7265625" customWidth="1"/>
     <col min="4" max="4" width="33.90625" customWidth="1"/>
     <col min="5" max="5" width="46.36328125" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="7" max="7" width="39.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.6">
@@ -596,69 +647,103 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="G5" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="G6" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="G7" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="G8" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="G9" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="G10" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="G12" s="5"/>

</xml_diff>